<commit_message>
Removed hardcoding of tokens and variables by parameterizing them and defining them in a .env file
</commit_message>
<xml_diff>
--- a/data_exports/enrollments_cleaned_1995626.xlsx
+++ b/data_exports/enrollments_cleaned_1995626.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,13 +539,13 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45902.12519675926</v>
+        <v>45985.02449074074</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8525</v>
+        <v>7.795277777777778</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -565,24 +565,24 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>66.89</t>
+          <t>87.71</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>6.37</t>
+          <t>59.29</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>66.89</t>
+          <t>89.41</t>
         </is>
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>6.37</t>
+          <t>73.94</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr"/>
@@ -602,13 +602,13 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45902.85973379629</v>
+        <v>45987.13950231481</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>4.203333333333333</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -628,24 +628,24 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>50.25</t>
+          <t>98.82</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>3.18</t>
+          <t>70.66</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>50.25</t>
+          <t>97.84</t>
         </is>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>3.18</t>
+          <t>84.61</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr"/>
@@ -665,13 +665,13 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45902.11071759259</v>
+        <v>45985.12440972222</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5522222222222222</v>
+        <v>5.04</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -691,24 +691,24 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>98.39</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>72.11</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.89</t>
         </is>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>86.41</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr"/>
@@ -728,13 +728,13 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45902.68399305556</v>
+        <v>45985.01984953704</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>1.391388888888889</v>
+        <v>5.435277777777777</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -754,24 +754,24 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>93.98</t>
         </is>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>67.10</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>94.21</t>
         </is>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>81.40</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
@@ -791,13 +791,13 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45902.72121527778</v>
+        <v>45985.65748842592</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>2.378055555555556</v>
+        <v>6.231666666666666</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -817,24 +817,24 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>100.56</t>
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>74.93</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>100.09</t>
         </is>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>89.58</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45901.28745370371</v>
+        <v>45986.01084490741</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>0.165</v>
+        <v>4.511666666666667</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -880,24 +880,24 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>95.15</t>
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>68.38</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>95.56</t>
         </is>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>83.03</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr"/>
@@ -917,13 +917,13 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45902.77334490741</v>
+        <v>45988.75021990741</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8672222222222222</v>
+        <v>4.443611111111111</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -943,24 +943,24 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>72.64</t>
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>54.43</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>76.34</t>
         </is>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>68.73</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr"/>
@@ -980,13 +980,13 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45902.81310185185</v>
+        <v>45988.73768518519</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4966666666666666</v>
+        <v>2.865277777777778</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1006,24 +1006,24 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>94.12</t>
         </is>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>61.74</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>92.71</t>
         </is>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>74.62</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr"/>
@@ -1043,13 +1043,13 @@
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>45902.76210648148</v>
+        <v>45988.15283564815</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8302777777777778</v>
+        <v>7.746388888888889</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1069,24 +1069,24 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>89.42</t>
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>58.63</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>89.64</t>
         </is>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>72.23</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr"/>
@@ -1106,13 +1106,13 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>45902.78489583333</v>
+        <v>45986.08052083333</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1552777777777778</v>
+        <v>1.785555555555556</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1132,24 +1132,24 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>83.39</t>
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>57.13</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>81.82</t>
         </is>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>68.20</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr"/>
@@ -1169,13 +1169,13 @@
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>45894.92821759259</v>
+        <v>45986.0827199074</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>1.608333333333333</v>
+        <v>8.831944444444444</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1195,24 +1195,24 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>82.49</t>
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>55.58</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>83.88</t>
         </is>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>69.18</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr"/>
@@ -1232,13 +1232,13 @@
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>45898.11603009259</v>
+        <v>45988.27900462963</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>8.896944444444445</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1258,24 +1258,24 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>90.33</t>
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>64.44</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>88.71</t>
         </is>
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>76.56</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr"/>
@@ -1295,13 +1295,13 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>45898.63965277778</v>
+        <v>45985.03459490741</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
-        <v>0.4552777777777778</v>
+        <v>3.428888888888889</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1321,31 +1321,31 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.44</t>
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>64.38</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.48</t>
         </is>
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>79.03</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5465667</v>
+        <v>5258113</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1358,13 +1358,13 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>45894.91866898148</v>
+        <v>45987.125625</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1572222222222222</v>
+        <v>5.530833333333334</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1378,37 +1378,37 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>U56203324</t>
+          <t>U34021070</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>87.68</t>
         </is>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>62.50</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>89.78</t>
         </is>
       </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>77.50</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>5258113</v>
+        <v>5519299</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1421,13 +1421,13 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>45902.65530092592</v>
+        <v>45986.64373842593</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
-        <v>1.328888888888889</v>
+        <v>6.4675</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1441,37 +1441,37 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>U34021070</t>
+          <t>U62347233</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.40</t>
         </is>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>69.60</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.44</t>
         </is>
       </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>84.25</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5519299</v>
+        <v>5458325</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1484,13 +1484,13 @@
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>45902.70173611111</v>
+        <v>45985.02575231482</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3786111111111111</v>
+        <v>8.159722222222221</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1504,37 +1504,37 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>U62347233</t>
+          <t>U91347090</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>94.18</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>69.17</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>93.99</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>83.12</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>5458325</v>
+        <v>5435739</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1547,13 +1547,13 @@
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>45902.67642361111</v>
+        <v>45988.84925925926</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5475</v>
+        <v>4.116388888888889</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1567,37 +1567,37 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>U91347090</t>
+          <t>U80777927</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>91.86</t>
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>67.08</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>90.14</t>
         </is>
       </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>79.28</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>5435739</v>
+        <v>5419653</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1610,13 +1610,13 @@
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>45902.86336805556</v>
+        <v>45988.84106481481</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5419444444444445</v>
+        <v>6.103333333333333</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1630,37 +1630,37 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>U80777927</t>
+          <t>U06354603</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>84.82</t>
         </is>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>60.42</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>79.45</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>68.42</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>5419653</v>
+        <v>5477723</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1673,13 +1673,13 @@
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>45902.70894675926</v>
+        <v>45987.69482638889</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>2.061666666666667</v>
+        <v>5.77</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1693,37 +1693,37 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>U06354603</t>
+          <t>U48845422</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>87.62</t>
         </is>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>62.46</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>88.53</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>76.41</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>5477723</v>
+        <v>5445017</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1736,13 +1736,13 @@
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>45902.65538194445</v>
+        <v>45985.72358796297</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
-        <v>0.8916666666666667</v>
+        <v>4.957222222222223</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1756,37 +1756,37 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>U48845422</t>
+          <t>U65990664</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>93.06</t>
         </is>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>64.90</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>94.20</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>79.90</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>5445017</v>
+        <v>5516889</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1799,13 +1799,13 @@
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>45897.13681712963</v>
+        <v>45980.66320601852</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4855555555555556</v>
+        <v>7.455</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1819,37 +1819,37 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>U65990664</t>
+          <t>U73781108</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>100.87</t>
         </is>
       </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>72.48</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>99.97</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>86.78</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>5516889</v>
+        <v>5477505</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1862,13 +1862,13 @@
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>45901.99901620371</v>
+        <v>45985.18728009259</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
-        <v>1.001944444444445</v>
+        <v>3.095</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1882,37 +1882,37 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>U73781108</t>
+          <t>U46466015</t>
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>49.52</t>
         </is>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>34.65</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>55.73</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>47.55</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>5477505</v>
+        <v>5497293</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1925,13 +1925,13 @@
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>45902.65850694444</v>
+        <v>45987.86027777778</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.7497222222222222</v>
+        <v>13.24666666666667</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1945,37 +1945,37 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>U46466015</t>
+          <t>U14127130</t>
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>93.26</t>
         </is>
       </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>63.03</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>93.60</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>77.33</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>5497293</v>
+        <v>5546537</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1988,13 +1988,13 @@
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>45901.18234953703</v>
+        <v>45986.77039351852</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1080555555555556</v>
+        <v>3.143611111111111</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -2008,37 +2008,37 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>U14127130</t>
+          <t>U95219941</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>91.40</t>
         </is>
       </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>66.77</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>92.04</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>81.07</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>5546537</v>
+        <v>5237579</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2051,13 +2051,13 @@
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45894.7758912037</v>
+        <v>45981.0595949074</v>
       </c>
       <c r="E26" t="n">
         <v>7</v>
       </c>
       <c r="F26" t="n">
-        <v>0.07083333333333333</v>
+        <v>3.513055555555555</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -2071,37 +2071,37 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>U95219941</t>
+          <t>U88462095</t>
         </is>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>31.42</t>
         </is>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>19.38</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>40.69</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>32.26</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>5237579</v>
+        <v>5457615</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2114,13 +2114,13 @@
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>45902.66005787037</v>
+        <v>45985.88290509259</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>0.4869444444444445</v>
+        <v>3.6875</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -2134,37 +2134,37 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>U88462095</t>
+          <t>U22087117</t>
         </is>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>66.03</t>
         </is>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>41.37</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>63.86</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>49.37</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>5457615</v>
+        <v>5455083</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2177,13 +2177,13 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>45902.13971064815</v>
+        <v>45981.73875</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
-        <v>0.8855555555555555</v>
+        <v>2.756666666666667</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -2197,37 +2197,37 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>U22087117</t>
+          <t>U13152977</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>35.89</t>
         </is>
       </c>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>19.63</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>38.86</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>27.63</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>5455083</v>
+        <v>5450695</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2240,13 +2240,13 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>45902.80994212963</v>
+        <v>45985.16921296297</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>0.3291666666666667</v>
+        <v>3.445277777777778</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -2260,37 +2260,37 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>U13152977</t>
+          <t>U85026645</t>
         </is>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>58.10</t>
         </is>
       </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>35.18</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>53.15</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>39.54</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>5450695</v>
+        <v>5546975</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -2303,13 +2303,13 @@
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>45902.86197916666</v>
+        <v>45986.07067129629</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
-        <v>0.7211111111111111</v>
+        <v>6.638888888888889</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -2323,37 +2323,37 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>U85026645</t>
+          <t>U20325003</t>
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>91.20</t>
         </is>
       </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>68.73</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>92.26</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>83.38</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>5546975</v>
+        <v>5359861</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2366,13 +2366,13 @@
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>45902.77417824074</v>
+        <v>45987.08039351852</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>0.6233333333333333</v>
+        <v>4.451944444444444</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -2386,37 +2386,37 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>U20325003</t>
+          <t>U82917225</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>81.08</t>
         </is>
       </c>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>57.24</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>83.41</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>71.54</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>5359861</v>
+        <v>5452619</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2429,13 +2429,13 @@
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>45902.69916666667</v>
+        <v>45988.8481712963</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.03944444444444444</v>
+        <v>16.50027777777778</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -2449,37 +2449,37 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>U82917225</t>
+          <t>U77632975</t>
         </is>
       </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>68.66</t>
         </is>
       </c>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>47.46</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>72.41</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>61.06</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>5452619</v>
+        <v>5445877</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2492,13 +2492,13 @@
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>45897.84465277778</v>
+        <v>45985.01997685185</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>0.8972222222222223</v>
+        <v>4.878888888888889</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2512,37 +2512,37 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>U77632975</t>
+          <t>U87068871</t>
         </is>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>17.09</t>
         </is>
       </c>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>10.17</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>22.63</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>17.45</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>5445877</v>
+        <v>5452411</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -2555,13 +2555,13 @@
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>45899.11885416666</v>
+        <v>45987.02815972222</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>3.873055555555556</v>
+        <v>3.841666666666667</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -2575,37 +2575,37 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>U87068871</t>
+          <t>U01739412</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>41.35</t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>24.86</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>49.77</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>38.81</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>5452411</v>
+        <v>5551387</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2618,13 +2618,13 @@
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>45897.816875</v>
+        <v>45986.80350694444</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>0.4461111111111111</v>
+        <v>4.252777777777778</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2638,41 +2638,41 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>U01739412</t>
+          <t>U74867618</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.53</t>
         </is>
       </c>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>70.21</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.17</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>84.51</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>5551387</v>
+        <v>5578501</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>StudentEnrollment</t>
+          <t>StudentViewEnrollment</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2681,14 +2681,14 @@
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>45902.65546296296</v>
+        <v>45901.19568287037</v>
       </c>
       <c r="E36" t="n">
+        <v>87</v>
+      </c>
+      <c r="F36" t="n">
         <v>0</v>
       </c>
-      <c r="F36" t="n">
-        <v>0.8005555555555556</v>
-      </c>
       <c r="G36" t="inlineStr">
         <is>
           <t>CGS2100.901F25</t>
@@ -2699,11 +2699,7 @@
           <t>CGS2100.901F25</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>U74867618</t>
-        </is>
-      </c>
+      <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
@@ -2713,7 +2709,7 @@
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>5.00</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -2724,33 +2720,33 @@
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>13.00</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>5578501</v>
+        <v>5202271</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>StudentViewEnrollment</t>
+          <t>TaEnrollment</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>StudentEnrollment</t>
+          <t>TaEnrollment</t>
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>45901.19568287037</v>
+        <v>45977.91584490741</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>5.551666666666667</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -2762,46 +2758,42 @@
           <t>CGS2100.901F25</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>U44677914</t>
+        </is>
+      </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
+      <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
+      <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>5202271</v>
+        <v>964585</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>TaEnrollment</t>
+          <t>TeacherEnrollment</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TaEnrollment</t>
+          <t>TeacherEnrollment</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>45902.69370370371</v>
+        <v>45988.94826388889</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.4294444444444445</v>
+        <v>5.4975</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2815,7 +2807,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>U44677914</t>
+          <t>U84383097</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
@@ -2827,53 +2819,6 @@
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
     </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>964585</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>TeacherEnrollment</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>TeacherEnrollment</t>
-        </is>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>45902.86809027778</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>1.5075</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>CGS2100.901F25</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>CGS2100.901F25</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>U84383097</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>